<commit_message>
All Templates Are Entered
</commit_message>
<xml_diff>
--- a/digital_inputs.xlsx
+++ b/digital_inputs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UserData\lanzaa\Documents\GitHub\Flask_Sites\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B05759F7-FA2B-426D-9FC8-DA686EF91270}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44CC82D8-7DB5-434F-AAAF-FB8075BE6169}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -550,7 +550,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M1" sqref="M1:M1048576"/>
+      <selection pane="topRight" activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -711,13 +711,13 @@
         <v>21</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="K3" s="6" t="s">
         <v>21</v>

</xml_diff>